<commit_message>
Ist commit 15-01-2020 11.19am
</commit_message>
<xml_diff>
--- a/CluthaSections.xlsx
+++ b/CluthaSections.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="141">
   <si>
     <t>C45</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>C31B</t>
-  </si>
-  <si>
-    <t>a change</t>
   </si>
   <si>
     <t>C31C</t>
@@ -448,11 +445,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -471,15 +468,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -494,15 +497,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -518,7 +513,23 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -526,14 +537,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -547,39 +551,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -592,10 +566,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -606,6 +581,28 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -616,187 +613,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -807,6 +804,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -835,54 +847,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -899,6 +863,30 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -907,153 +895,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1643,7 +1640,7 @@
   <dimension ref="A2:U186"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -1891,15 +1888,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="C19" t="s">
         <v>29</v>
-      </c>
-      <c r="G19" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1907,7 +1901,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1915,7 +1909,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1923,7 +1917,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1931,7 +1925,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1939,7 +1933,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1947,7 +1941,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1955,7 +1949,7 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1963,7 +1957,7 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1971,7 +1965,7 @@
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1979,7 +1973,7 @@
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1987,7 +1981,7 @@
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1995,7 +1989,7 @@
         <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -2003,7 +1997,7 @@
         <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -2011,7 +2005,7 @@
         <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -2019,7 +2013,7 @@
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -2027,7 +2021,7 @@
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -2035,7 +2029,7 @@
         <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -2043,7 +2037,7 @@
         <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -2051,7 +2045,7 @@
         <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -2059,7 +2053,7 @@
         <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -2067,7 +2061,7 @@
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -2075,7 +2069,7 @@
         <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -2083,7 +2077,7 @@
         <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -2091,7 +2085,7 @@
         <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -2099,7 +2093,7 @@
         <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -2107,7 +2101,7 @@
         <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -2115,7 +2109,7 @@
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -2123,7 +2117,7 @@
         <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -2131,7 +2125,7 @@
         <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -2139,7 +2133,7 @@
         <v>48</v>
       </c>
       <c r="C49" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -2147,7 +2141,7 @@
         <v>49</v>
       </c>
       <c r="C50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -2155,7 +2149,7 @@
         <v>50</v>
       </c>
       <c r="C51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -2163,7 +2157,7 @@
         <v>51</v>
       </c>
       <c r="C52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -2171,7 +2165,7 @@
         <v>52</v>
       </c>
       <c r="C53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -2179,7 +2173,7 @@
         <v>53</v>
       </c>
       <c r="C54" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -2187,7 +2181,7 @@
         <v>54</v>
       </c>
       <c r="C55" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -2195,7 +2189,7 @@
         <v>55</v>
       </c>
       <c r="C56" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -2203,7 +2197,7 @@
         <v>56</v>
       </c>
       <c r="C57" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -2211,7 +2205,7 @@
         <v>57</v>
       </c>
       <c r="C58" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -2219,7 +2213,7 @@
         <v>58</v>
       </c>
       <c r="C59" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -2227,7 +2221,7 @@
         <v>59</v>
       </c>
       <c r="C60" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -2235,7 +2229,7 @@
         <v>60</v>
       </c>
       <c r="C61" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -2243,7 +2237,7 @@
         <v>61</v>
       </c>
       <c r="C62" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -2251,7 +2245,7 @@
         <v>62</v>
       </c>
       <c r="C63" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -2259,7 +2253,7 @@
         <v>63</v>
       </c>
       <c r="C64" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -2267,7 +2261,7 @@
         <v>64</v>
       </c>
       <c r="C65" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -2275,7 +2269,7 @@
         <v>65</v>
       </c>
       <c r="C66" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -2283,7 +2277,7 @@
         <v>66</v>
       </c>
       <c r="C67" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -2291,7 +2285,7 @@
         <v>67</v>
       </c>
       <c r="C68" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -2299,7 +2293,7 @@
         <v>68</v>
       </c>
       <c r="C69" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -2307,7 +2301,7 @@
         <v>69</v>
       </c>
       <c r="C70" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2315,10 +2309,10 @@
         <v>70</v>
       </c>
       <c r="C71" t="s">
+        <v>81</v>
+      </c>
+      <c r="D71" t="s">
         <v>82</v>
-      </c>
-      <c r="D71" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -2326,7 +2320,7 @@
         <v>71</v>
       </c>
       <c r="C72" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -2334,7 +2328,7 @@
         <v>72</v>
       </c>
       <c r="C73" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -2342,7 +2336,7 @@
         <v>73</v>
       </c>
       <c r="C74" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -2350,7 +2344,7 @@
         <v>74</v>
       </c>
       <c r="C75" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -2358,7 +2352,7 @@
         <v>75</v>
       </c>
       <c r="C76" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -2366,7 +2360,7 @@
         <v>76</v>
       </c>
       <c r="C77" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2374,7 +2368,7 @@
         <v>77</v>
       </c>
       <c r="C78" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -2382,7 +2376,7 @@
         <v>78</v>
       </c>
       <c r="C79" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -2390,7 +2384,7 @@
         <v>79</v>
       </c>
       <c r="C80" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -2398,7 +2392,7 @@
         <v>80</v>
       </c>
       <c r="C81" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -2406,7 +2400,7 @@
         <v>81</v>
       </c>
       <c r="C82" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -2414,7 +2408,7 @@
         <v>82</v>
       </c>
       <c r="C83" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -2422,7 +2416,7 @@
         <v>83</v>
       </c>
       <c r="C84" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -2430,7 +2424,7 @@
         <v>84</v>
       </c>
       <c r="C85" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -2438,7 +2432,7 @@
         <v>85</v>
       </c>
       <c r="C86" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -2446,7 +2440,7 @@
         <v>86</v>
       </c>
       <c r="C87" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -2454,7 +2448,7 @@
         <v>87</v>
       </c>
       <c r="C88" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="89" spans="1:3">
@@ -2462,7 +2456,7 @@
         <v>88</v>
       </c>
       <c r="C89" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -2470,7 +2464,7 @@
         <v>89</v>
       </c>
       <c r="C90" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="91" spans="1:3">
@@ -2478,7 +2472,7 @@
         <v>90</v>
       </c>
       <c r="C91" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -2486,7 +2480,7 @@
         <v>91</v>
       </c>
       <c r="C92" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -2494,7 +2488,7 @@
         <v>92</v>
       </c>
       <c r="C93" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -2502,7 +2496,7 @@
         <v>93</v>
       </c>
       <c r="C94" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -2510,7 +2504,7 @@
         <v>94</v>
       </c>
       <c r="C95" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -2518,7 +2512,7 @@
         <v>95</v>
       </c>
       <c r="C96" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -2526,7 +2520,7 @@
         <v>96</v>
       </c>
       <c r="C97" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2534,15 +2528,15 @@
         <v>97</v>
       </c>
       <c r="C98" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D98" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="186" spans="21:21">
       <c r="U186" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2565,272 +2559,272 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>